<commit_message>
fix mapping duplicates [GEAR-182] (#26)
* Fix mapping config for duplicate  keys [GEAR-182]

- Config mapping can define multiple keys pointing to same
value or list of values.
- key_from_flywheel now returns tupple of list of matching values
- fix broken tests and add new

* fix typo in example file

* restore circleci config, update dockerfile, cleanup

* add circleci badge

* fix test name duplicate (test_create_missing_error)
</commit_message>
<xml_diff>
--- a/examples/transfer-log.xlsx
+++ b/examples/transfer-log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/cids/data/shared/Curation POC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaspannetier/code/gears/flywheel-apps/GRP-5-transfer-log-report/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B34B4F6-CB0A-6248-A463-5DC9B53F215B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C309F1-3F12-B146-90B3-90697DEAB6AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2840" windowWidth="30440" windowHeight="16940" xr2:uid="{F0DD9B24-E4DC-4947-B5F7-A733744F13F5}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -151,9 +150,6 @@
     <t>MR - Nov 20, 2005</t>
   </si>
   <si>
-    <t>MR - Jan 02 2005</t>
-  </si>
-  <si>
     <t>MR - Mar 28, 2005</t>
   </si>
   <si>
@@ -212,6 +208,9 @@
   </si>
   <si>
     <t>MR - Oct 02, 2006</t>
+  </si>
+  <si>
+    <t>MR - Jan 02, 2005</t>
   </si>
 </sst>
 </file>
@@ -581,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD0E26B-FBE1-4247-AA77-950C66F78CEA}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,7 +969,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -984,12 +983,12 @@
         <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1">
         <v>11701</v>
@@ -998,12 +997,12 @@
         <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1">
         <v>11701</v>
@@ -1012,12 +1011,12 @@
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1">
         <v>11701</v>
@@ -1026,12 +1025,12 @@
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1">
         <v>11701</v>
@@ -1040,12 +1039,12 @@
         <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1">
         <v>11701</v>
@@ -1054,12 +1053,12 @@
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1">
         <v>11701</v>
@@ -1068,12 +1067,12 @@
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1">
         <v>11701</v>
@@ -1082,12 +1081,12 @@
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1">
         <v>11701</v>
@@ -1096,12 +1095,12 @@
         <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1">
         <v>11701</v>
@@ -1110,12 +1109,12 @@
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>11853</v>
@@ -1124,12 +1123,12 @@
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38">
         <v>11853</v>
@@ -1138,12 +1137,12 @@
         <v>7</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39">
         <v>11853</v>
@@ -1152,12 +1151,12 @@
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>11853</v>
@@ -1166,12 +1165,12 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41">
         <v>11853</v>
@@ -1180,12 +1179,12 @@
         <v>13</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <v>11853</v>
@@ -1194,12 +1193,12 @@
         <v>15</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <v>11853</v>
@@ -1208,12 +1207,12 @@
         <v>16</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44">
         <v>11853</v>
@@ -1222,12 +1221,12 @@
         <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45">
         <v>11853</v>
@@ -1236,7 +1235,7 @@
         <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>